<commit_message>
Added Lua Config Scripting
</commit_message>
<xml_diff>
--- a/examples_sheets/example-timetable_school.xlsx
+++ b/examples_sheets/example-timetable_school.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB3C0BE-D96F-4193-A13D-99F1BFB848A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CD9C7C-5025-48D9-B72B-1546D4587BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" activeTab="4" xr2:uid="{41FF037C-E733-4109-8018-268BF2C7ACEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" activeTab="3" xr2:uid="{41FF037C-E733-4109-8018-268BF2C7ACEB}"/>
   </bookViews>
   <sheets>
     <sheet name="district" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="319">
   <si>
     <t>District Cells</t>
   </si>
@@ -1594,10 +1594,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:BE20"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="AW1" sqref="AW1"/>
+      <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2049,6 +2049,9 @@
       <c r="AT1" s="22"/>
       <c r="AU1" s="22"/>
       <c r="AV1" s="22"/>
+      <c r="AW1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:57" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -2146,9 +2149,6 @@
       </c>
       <c r="AF2" s="1">
         <v>0</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="AX2" s="23" t="s">
         <v>2</v>
@@ -3140,7 +3140,7 @@
   <dimension ref="A1:AG196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3153,153 +3153,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="4"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="AG1" s="4"/>
     </row>
     <row r="2" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
+      <c r="D2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
     </row>
     <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25" t="s">
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="25"/>
+      <c r="Q3" s="24"/>
       <c r="R3" s="26" t="s">
         <v>18</v>
       </c>
       <c r="S3" s="26"/>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25" t="s">
+      <c r="U3" s="24"/>
+      <c r="V3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25" t="s">
+      <c r="W3" s="24"/>
+      <c r="X3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25" t="s">
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25" t="s">
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25" t="s">
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE3" s="24"/>
     </row>
     <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
@@ -15266,6 +15265,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:Y3"/>
@@ -15282,9 +15284,6 @@
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -15293,10 +15292,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614FD235-4236-4207-9A64-880D49E7EAB5}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15307,15 +15306,18 @@
     <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-    </row>
-    <row r="2" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>228</v>
       </c>
@@ -15329,7 +15331,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -15341,7 +15343,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -15353,7 +15355,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -15365,13 +15367,13 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
@@ -15381,7 +15383,7 @@
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -15391,13 +15393,13 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -15407,7 +15409,7 @@
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -15417,7 +15419,7 @@
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -15427,13 +15429,13 @@
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
@@ -15443,12 +15445,12 @@
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -15519,8 +15521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B013458-3FFF-4982-A44F-299B41089B86}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15539,18 +15541,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -16056,8 +16061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144123B6-861A-40B0-B710-7CC8C00594E2}">
   <dimension ref="A1:AF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16067,149 +16072,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:32" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
     </row>
     <row r="3" spans="1:32" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25" t="s">
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25" t="s">
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25" t="s">
+      <c r="S3" s="24"/>
+      <c r="T3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25" t="s">
+      <c r="U3" s="24"/>
+      <c r="V3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25" t="s">
+      <c r="W3" s="24"/>
+      <c r="X3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25" t="s">
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25" t="s">
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25" t="s">
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE3" s="24"/>
     </row>
     <row r="4" spans="1:32" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="6" t="s">
         <v>271</v>
       </c>
@@ -17589,6 +17594,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="X3:Y3"/>
@@ -17605,9 +17613,6 @@
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>